<commit_message>
Prior to modification of _evaluationDate
</commit_message>
<xml_diff>
--- a/Cephei.XL/FixedRateBond.xlsx
+++ b/Cephei.XL/FixedRateBond.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\source\repos\Cephei2\Cephei.XL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E817C3-C7EE-4F6E-9A25-8D4C66261FF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B1E57F-5248-4559-A2FF-E4181A5518BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="120" windowWidth="38380" windowHeight="20880" xr2:uid="{347D0D25-E149-495F-B150-3BFF05A50DF3}"/>
   </bookViews>
@@ -182,16 +182,7 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="rtdsrv.1b13c30b514c4f3c9ded145fb5c22f88">
-      <tp>
-        <v>44137</v>
-        <stp/>
-        <stp>-PriceDay</stp>
-        <stp/>
-        <tr r="B5" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.dd435e9a7dad46f6beeab89e65cf6111">
+    <main first="rtdsrv.7d414220322c4792bc225a5c77672862">
       <tp t="s">
         <v>-Coupon</v>
         <stp/>
@@ -200,7 +191,16 @@
         <tr r="D19" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.dd435e9a7dad46f6beeab89e65cf6111">
+    <main first="rtdsrv.1748d324e7d043fbb53bf0573bb9a9a8">
+      <tp>
+        <v>7408833984.0674105</v>
+        <stp/>
+        <stp>NPV</stp>
+        <stp/>
+        <tr r="B23" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.7d414220322c4792bc225a5c77672862">
       <tp t="s">
         <v>-DayCount</v>
         <stp/>
@@ -209,50 +209,25 @@
         <tr r="D6" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.dd435e9a7dad46f6beeab89e65cf6111">
-      <tp t="s">
-        <v>-clock</v>
-        <stp/>
-        <stp>-clock</stp>
-        <stp>44137</stp>
-        <tr r="D3" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>CleanPrice</v>
-        <stp/>
-        <stp>CleanPrice</stp>
-        <stp>-1893055664</stp>
-        <tr r="D24" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.dd435e9a7dad46f6beeab89e65cf6111">
-      <tp t="s">
-        <v>-Schedule</v>
-        <stp/>
-        <stp>-Schedule</stp>
-        <stp>2041998490</stp>
-        <tr r="D17" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.dd435e9a7dad46f6beeab89e65cf6111">
-      <tp t="s">
-        <v>+Maturity</v>
-        <stp/>
-        <stp>+Maturity</stp>
-        <stp>1609061136</stp>
-        <tr r="D11" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.dd435e9a7dad46f6beeab89e65cf6111">
-      <tp t="s">
-        <v>+FixedAmount</v>
-        <stp/>
-        <stp>+FixedAmount</stp>
-        <stp>1093567616</stp>
-        <tr r="D16" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.dd435e9a7dad46f6beeab89e65cf6111">
+    <main first="rtdsrv.7d414220322c4792bc225a5c77672862">
+      <tp t="s">
+        <v>NPV</v>
+        <stp/>
+        <stp>NPV</stp>
+        <stp>46212239</stp>
+        <tr r="D23" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.7d414220322c4792bc225a5c77672862">
+      <tp t="s">
+        <v>Clock</v>
+        <stp/>
+        <stp>Clock</stp>
+        <stp>0</stp>
+        <tr r="D9" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.7d414220322c4792bc225a5c77672862">
       <tp t="s">
         <v>-ExCoupon</v>
         <stp/>
@@ -260,13 +235,8 @@
         <stp>0</stp>
         <tr r="D7" s="1"/>
       </tp>
-      <tp t="s">
-        <v>-PriceDay</v>
-        <stp/>
-        <stp>-PriceDay</stp>
-        <stp>1479526416</stp>
-        <tr r="D5" s="1"/>
-      </tp>
+    </main>
+    <main first="rtdsrv.7d414220322c4792bc225a5c77672862">
       <tp t="s">
         <v>Today</v>
         <stp/>
@@ -276,34 +246,32 @@
         <tr r="D2" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.1b13c30b514c4f3c9ded145fb5c22f88">
-      <tp>
-        <v>10000770109.289618</v>
-        <stp/>
-        <stp>Cash</stp>
-        <stp/>
-        <tr r="B22" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.dd435e9a7dad46f6beeab89e65cf6111">
-      <tp t="s">
-        <v>Clock</v>
-        <stp/>
-        <stp>Clock</stp>
-        <stp>0</stp>
-        <tr r="D9" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.dd435e9a7dad46f6beeab89e65cf6111">
-      <tp t="s">
-        <v>DirtyPrice</v>
-        <stp/>
-        <stp>DirtyPrice</stp>
-        <stp>-1893055664</stp>
-        <tr r="D25" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.dd435e9a7dad46f6beeab89e65cf6111">
+    <main first="rtdsrv.7d414220322c4792bc225a5c77672862">
+      <tp t="s">
+        <v>+FixedAmount</v>
+        <stp/>
+        <stp>+FixedAmount</stp>
+        <stp>1093567616</stp>
+        <tr r="D16" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>+Maturity</v>
+        <stp/>
+        <stp>+Maturity</stp>
+        <stp>-1235442928</stp>
+        <tr r="D11" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.7d414220322c4792bc225a5c77672862">
+      <tp t="s">
+        <v>clock</v>
+        <stp/>
+        <stp>clock</stp>
+        <stp>-367521373</stp>
+        <tr r="A3" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.7d414220322c4792bc225a5c77672862">
       <tp t="s">
         <v>-Calendar</v>
         <stp/>
@@ -312,43 +280,48 @@
         <tr r="D4" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.dd435e9a7dad46f6beeab89e65cf6111">
-      <tp t="s">
-        <v>clock</v>
-        <stp/>
-        <stp>clock</stp>
-        <stp>44137</stp>
-        <tr r="A3" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.1b13c30b514c4f3c9ded145fb5c22f88">
+    <main first="rtdsrv.7d414220322c4792bc225a5c77672862">
+      <tp t="s">
+        <v>Quote</v>
+        <stp/>
+        <stp>Quote</stp>
+        <stp>-736385303</stp>
+        <tr r="D13" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.1748d324e7d043fbb53bf0573bb9a9a8">
       <tp>
-        <v>740883.40386987466</v>
+        <v>44152.642362627317</v>
+        <stp/>
+        <stp>Clock</stp>
+        <stp/>
+        <tr r="D9" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.1748d324e7d043fbb53bf0573bb9a9a8">
+      <tp>
+        <v>44152</v>
+        <stp/>
+        <stp>Today</stp>
+        <stp/>
+        <tr r="B2" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.7d414220322c4792bc225a5c77672862">
+      <tp t="s">
+        <v>-PriceDay</v>
+        <stp/>
+        <stp>-PriceDay</stp>
+        <stp>752134320</stp>
+        <tr r="D5" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>CleanPrice</v>
         <stp/>
         <stp>CleanPrice</stp>
-        <stp/>
-        <tr r="B24" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.1b13c30b514c4f3c9ded145fb5c22f88">
-      <tp>
-        <v>7408834038.6987467</v>
-        <stp/>
-        <stp>NPV</stp>
-        <stp/>
-        <tr r="B23" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.dd435e9a7dad46f6beeab89e65cf6111">
-      <tp t="s">
-        <v>-Bond</v>
-        <stp/>
-        <stp>-Bond</stp>
-        <stp>569985074</stp>
-        <tr r="D18" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.dd435e9a7dad46f6beeab89e65cf6111">
+        <stp>46212239</stp>
+        <tr r="D24" s="1"/>
+      </tp>
       <tp t="s">
         <v>Frequency</v>
         <stp/>
@@ -357,43 +330,70 @@
         <tr r="D12" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.dd435e9a7dad46f6beeab89e65cf6111">
-      <tp t="s">
-        <v>Cash</v>
-        <stp/>
-        <stp>Cash</stp>
-        <stp>-1893055664</stp>
-        <tr r="D22" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.1b13c30b514c4f3c9ded145fb5c22f88">
+    <main first="rtdsrv.7d414220322c4792bc225a5c77672862">
+      <tp t="s">
+        <v>-Bond</v>
+        <stp/>
+        <stp>-Bond</stp>
+        <stp>-1401924820</stp>
+        <tr r="D18" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.1748d324e7d043fbb53bf0573bb9a9a8">
       <tp>
-        <v>740883.40386987466</v>
+        <v>740883.39840674109</v>
+        <stp/>
+        <stp>CleanPrice</stp>
+        <stp/>
+        <tr r="B24" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.7d414220322c4792bc225a5c77672862">
+      <tp t="s">
+        <v>DirtyPrice</v>
         <stp/>
         <stp>DirtyPrice</stp>
+        <stp>46212239</stp>
+        <tr r="D25" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.1748d324e7d043fbb53bf0573bb9a9a8">
+      <tp>
+        <v>740883.39840674109</v>
+        <stp/>
+        <stp>DirtyPrice</stp>
         <stp/>
         <tr r="B25" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.dd435e9a7dad46f6beeab89e65cf6111">
-      <tp t="s">
-        <v>NPV</v>
-        <stp/>
-        <stp>NPV</stp>
-        <stp>-1893055664</stp>
-        <tr r="D23" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.1b13c30b514c4f3c9ded145fb5c22f88">
+    <main first="rtdsrv.1748d324e7d043fbb53bf0573bb9a9a8">
       <tp>
-        <v>44137</v>
-        <stp/>
-        <stp>Today</stp>
-        <stp/>
-        <tr r="B2" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.dd435e9a7dad46f6beeab89e65cf6111">
+        <v>44152</v>
+        <stp/>
+        <stp>-PriceDay</stp>
+        <stp/>
+        <tr r="B5" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.7d414220322c4792bc225a5c77672862">
+      <tp t="s">
+        <v>-clock</v>
+        <stp/>
+        <stp>-clock</stp>
+        <stp>-367521373</stp>
+        <tr r="D3" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.7d414220322c4792bc225a5c77672862">
+      <tp t="s">
+        <v>-Engine</v>
+        <stp/>
+        <stp>-Engine</stp>
+        <stp>-1822597231</stp>
+        <tr r="D15" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.7d414220322c4792bc225a5c77672862">
       <tp t="s">
         <v>+Tenor</v>
         <stp/>
@@ -402,49 +402,47 @@
         <tr r="D10" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.1b13c30b514c4f3c9ded145fb5c22f88">
+    <main first="rtdsrv.7d414220322c4792bc225a5c77672862">
+      <tp t="s">
+        <v>-FlatForward</v>
+        <stp/>
+        <stp>-FlatForward</stp>
+        <stp>26205480</stp>
+        <tr r="D14" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.7d414220322c4792bc225a5c77672862">
+      <tp t="s">
+        <v>-Schedule</v>
+        <stp/>
+        <stp>-Schedule</stp>
+        <stp>1253469338</stp>
+        <tr r="D17" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.1748d324e7d043fbb53bf0573bb9a9a8">
       <tp>
-        <v>44137.098170567129</v>
-        <stp/>
-        <stp>Clock</stp>
-        <stp/>
-        <tr r="D9" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.dd435e9a7dad46f6beeab89e65cf6111">
-      <tp t="s">
-        <v>Quote</v>
-        <stp/>
-        <stp>Quote</stp>
-        <stp>-736385303</stp>
-        <tr r="D13" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.dd435e9a7dad46f6beeab89e65cf6111">
-      <tp t="s">
-        <v>-Engine</v>
-        <stp/>
-        <stp>-Engine</stp>
-        <stp>1487502897</stp>
-        <tr r="D15" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.dd435e9a7dad46f6beeab89e65cf6111">
+        <v>10000770054.644808</v>
+        <stp/>
+        <stp>Cash</stp>
+        <stp/>
+        <tr r="B22" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.7d414220322c4792bc225a5c77672862">
+      <tp t="s">
+        <v>Cash</v>
+        <stp/>
+        <stp>Cash</stp>
+        <stp>46212239</stp>
+        <tr r="D22" s="1"/>
+      </tp>
       <tp t="s">
         <v>-Settlement</v>
         <stp/>
         <stp>-Settlement</stp>
         <stp>0</stp>
         <tr r="D8" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.dd435e9a7dad46f6beeab89e65cf6111">
-      <tp t="s">
-        <v>-FlatForward</v>
-        <stp/>
-        <stp>-FlatForward</stp>
-        <stp>541987472</stp>
-        <tr r="D14" s="1"/>
       </tp>
     </main>
   </volType>
@@ -766,7 +764,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -799,7 +797,7 @@
       </c>
       <c r="B2" s="1">
         <f>+_xll._Value(A2)</f>
-        <v>44137</v>
+        <v>44152</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" t="str">
@@ -838,7 +836,7 @@
       </c>
       <c r="B5" s="1">
         <f>+_xll._Value(D5)</f>
-        <v>44137</v>
+        <v>44152</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
@@ -896,7 +894,7 @@
       </c>
       <c r="D9" s="2">
         <f>+_xll._Clock()</f>
-        <v>44137.098170567129</v>
+        <v>44152.642362627317</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -1053,7 +1051,7 @@
       </c>
       <c r="B22" s="6">
         <f>+_xll._Value(D22)</f>
-        <v>10000770109.289618</v>
+        <v>10000770054.644808</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" t="str">
@@ -1067,7 +1065,7 @@
       </c>
       <c r="B23" s="6">
         <f>+_xll._Value(D23)</f>
-        <v>7408834038.6987467</v>
+        <v>7408833984.0674105</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" t="str">
@@ -1081,7 +1079,7 @@
       </c>
       <c r="B24" s="6">
         <f>+_xll._Value(D24)</f>
-        <v>740883.40386987466</v>
+        <v>740883.39840674109</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" t="str">
@@ -1095,7 +1093,7 @@
       </c>
       <c r="B25" s="6">
         <f>+_xll._Value(D25)</f>
-        <v>740883.40386987466</v>
+        <v>740883.39840674109</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" t="str">

</xml_diff>

<commit_message>
Updated Generated code mapping
</commit_message>
<xml_diff>
--- a/Cephei.XL/FixedRateBond.xlsx
+++ b/Cephei.XL/FixedRateBond.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\source\repos\Cephei2\Cephei.XL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8500BEDA-5AA9-4C28-98B8-512BBDA8A7A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{084A8B1A-F29B-47A9-84F5-CA8FE46E7488}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="380" windowWidth="38400" windowHeight="21000" xr2:uid="{347D0D25-E149-495F-B150-3BFF05A50DF3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{347D0D25-E149-495F-B150-3BFF05A50DF3}"/>
   </bookViews>
   <sheets>
     <sheet name="FixedBond" sheetId="1" r:id="rId1"/>
@@ -182,43 +182,25 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="rtdsrv.0525cccb232d485c91876ecb77b7d8b2">
-      <tp t="s">
-        <v>Cash</v>
-        <stp/>
-        <stp>Cash</stp>
-        <stp>-1893055664</stp>
-        <tr r="D22" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.0525cccb232d485c91876ecb77b7d8b2">
-      <tp t="s">
-        <v>-Bond</v>
-        <stp/>
-        <stp>-Bond</stp>
-        <stp>-893206484</stp>
-        <tr r="D18" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.3519a603d24449b7954455d4a9ab6a31">
+    <main first="rtdsrv.5f13c665aaa54d02a8beae1c73f116fd">
       <tp>
-        <v>139.26501022498323</v>
-        <stp/>
-        <stp>DirtyPrice</stp>
-        <stp/>
-        <tr r="B25" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.3519a603d24449b7954455d4a9ab6a31">
-      <tp>
-        <v>139.26501022498323</v>
-        <stp/>
-        <stp>CleanPrice</stp>
-        <stp/>
-        <tr r="B24" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.0525cccb232d485c91876ecb77b7d8b2">
+        <v>44179</v>
+        <stp/>
+        <stp>-PriceDay</stp>
+        <stp/>
+        <tr r="B5" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.5bed24b1e93346e4ab5804fc2c77058c">
+      <tp t="s">
+        <v>Frequency</v>
+        <stp/>
+        <stp>Frequency</stp>
+        <stp>-272257755</stp>
+        <tr r="D12" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.5bed24b1e93346e4ab5804fc2c77058c">
       <tp t="s">
         <v>-FlatForward</v>
         <stp/>
@@ -227,7 +209,16 @@
         <tr r="D14" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.0525cccb232d485c91876ecb77b7d8b2">
+    <main first="rtdsrv.5f13c665aaa54d02a8beae1c73f116fd">
+      <tp>
+        <v>177.0109289617487</v>
+        <stp/>
+        <stp>Cash</stp>
+        <stp/>
+        <tr r="B22" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.5bed24b1e93346e4ab5804fc2c77058c">
       <tp t="s">
         <v>Today</v>
         <stp/>
@@ -237,7 +228,7 @@
         <tr r="D2" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.0525cccb232d485c91876ecb77b7d8b2">
+    <main first="rtdsrv.5bed24b1e93346e4ab5804fc2c77058c">
       <tp t="s">
         <v>-ExCoupon</v>
         <stp/>
@@ -246,7 +237,16 @@
         <tr r="D7" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.0525cccb232d485c91876ecb77b7d8b2">
+    <main first="rtdsrv.5bed24b1e93346e4ab5804fc2c77058c">
+      <tp t="s">
+        <v>-Settlement</v>
+        <stp/>
+        <stp>-Settlement</stp>
+        <stp>0</stp>
+        <tr r="D8" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.5bed24b1e93346e4ab5804fc2c77058c">
       <tp t="s">
         <v>Clock</v>
         <stp/>
@@ -255,202 +255,202 @@
         <tr r="D9" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.0525cccb232d485c91876ecb77b7d8b2">
+    <main first="rtdsrv.5bed24b1e93346e4ab5804fc2c77058c">
+      <tp t="s">
+        <v>+FixedAmount</v>
+        <stp/>
+        <stp>+FixedAmount</stp>
+        <stp>1079574528</stp>
+        <tr r="D16" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.5bed24b1e93346e4ab5804fc2c77058c">
+      <tp t="s">
+        <v>+Maturity</v>
+        <stp/>
+        <stp>+Maturity</stp>
+        <stp>1718322077</stp>
+        <tr r="D11" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.5bed24b1e93346e4ab5804fc2c77058c">
+      <tp t="s">
+        <v>-Engine</v>
+        <stp/>
+        <stp>-Engine</stp>
+        <stp>2035139617</stp>
+        <tr r="D15" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.5bed24b1e93346e4ab5804fc2c77058c">
+      <tp t="s">
+        <v>-clock</v>
+        <stp/>
+        <stp>-clock</stp>
+        <stp>-367521373</stp>
+        <tr r="D3" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.5bed24b1e93346e4ab5804fc2c77058c">
+      <tp t="s">
+        <v>-Calendar</v>
+        <stp/>
+        <stp>-Calendar</stp>
+        <stp>0</stp>
+        <tr r="D4" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.5bed24b1e93346e4ab5804fc2c77058c">
+      <tp t="s">
+        <v>+Tenor</v>
+        <stp/>
+        <stp>+Tenor</stp>
+        <stp>10</stp>
+        <tr r="D10" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.5bed24b1e93346e4ab5804fc2c77058c">
+      <tp t="s">
+        <v>Quote</v>
+        <stp/>
+        <stp>Quote</stp>
+        <stp>0</stp>
+        <tr r="D13" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.5bed24b1e93346e4ab5804fc2c77058c">
+      <tp t="s">
+        <v>-DayCount</v>
+        <stp/>
+        <stp>-DayCount</stp>
+        <stp>1443484981</stp>
+        <tr r="D6" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.5bed24b1e93346e4ab5804fc2c77058c">
+      <tp t="s">
+        <v>-Schedule</v>
+        <stp/>
+        <stp>-Schedule</stp>
+        <stp>2392593</stp>
+        <tr r="D17" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.5f13c665aaa54d02a8beae1c73f116fd">
+      <tp>
+        <v>139.26501022498323</v>
+        <stp/>
+        <stp>NPV</stp>
+        <stp/>
+        <tr r="B23" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.5f13c665aaa54d02a8beae1c73f116fd">
+      <tp>
+        <v>139.26501022498323</v>
+        <stp/>
+        <stp>CleanPrice</stp>
+        <stp/>
+        <tr r="B24" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.5bed24b1e93346e4ab5804fc2c77058c">
+      <tp t="s">
+        <v>-PriceDay</v>
+        <stp/>
+        <stp>-PriceDay</stp>
+        <stp>-1100403559</stp>
+        <tr r="D5" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.5bed24b1e93346e4ab5804fc2c77058c">
+      <tp t="s">
+        <v>-Bond</v>
+        <stp/>
+        <stp>-Bond</stp>
+        <stp>-893206484</stp>
+        <tr r="D18" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.5bed24b1e93346e4ab5804fc2c77058c">
+      <tp t="s">
+        <v>-Coupon</v>
+        <stp/>
+        <stp>-Coupon</stp>
+        <stp>561312938</stp>
+        <tr r="D19" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.5f13c665aaa54d02a8beae1c73f116fd">
+      <tp>
+        <v>139.26501022498323</v>
+        <stp/>
+        <stp>DirtyPrice</stp>
+        <stp/>
+        <tr r="B25" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.5bed24b1e93346e4ab5804fc2c77058c">
+      <tp t="s">
+        <v>Cash</v>
+        <stp/>
+        <stp>Cash</stp>
+        <stp>-1893055664</stp>
+        <tr r="D22" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.5bed24b1e93346e4ab5804fc2c77058c">
+      <tp t="s">
+        <v>DirtyPrice</v>
+        <stp/>
+        <stp>DirtyPrice</stp>
+        <stp>-1893055664</stp>
+        <tr r="D25" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.5f13c665aaa54d02a8beae1c73f116fd">
+      <tp>
+        <v>44179</v>
+        <stp/>
+        <stp>Today</stp>
+        <stp/>
+        <tr r="B2" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.5bed24b1e93346e4ab5804fc2c77058c">
+      <tp t="s">
+        <v>NPV</v>
+        <stp/>
+        <stp>NPV</stp>
+        <stp>-1893055664</stp>
+        <tr r="D23" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.5f13c665aaa54d02a8beae1c73f116fd">
+      <tp>
+        <v>44179.561450185189</v>
+        <stp/>
+        <stp>Clock</stp>
+        <stp/>
+        <tr r="D9" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.5bed24b1e93346e4ab5804fc2c77058c">
+      <tp t="s">
+        <v>CleanPrice</v>
+        <stp/>
+        <stp>CleanPrice</stp>
+        <stp>-1893055664</stp>
+        <tr r="D24" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.5bed24b1e93346e4ab5804fc2c77058c">
       <tp t="s">
         <v>clock</v>
         <stp/>
         <stp>clock</stp>
         <stp>-367521373</stp>
         <tr r="A3" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.0525cccb232d485c91876ecb77b7d8b2">
-      <tp t="s">
-        <v>+FixedAmount</v>
-        <stp/>
-        <stp>+FixedAmount</stp>
-        <stp>1079574528</stp>
-        <tr r="D16" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.0525cccb232d485c91876ecb77b7d8b2">
-      <tp t="s">
-        <v>-Settlement</v>
-        <stp/>
-        <stp>-Settlement</stp>
-        <stp>0</stp>
-        <tr r="D8" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.0525cccb232d485c91876ecb77b7d8b2">
-      <tp t="s">
-        <v>CleanPrice</v>
-        <stp/>
-        <stp>CleanPrice</stp>
-        <stp>-1893055664</stp>
-        <tr r="D24" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.3519a603d24449b7954455d4a9ab6a31">
-      <tp>
-        <v>44178</v>
-        <stp/>
-        <stp>Today</stp>
-        <stp/>
-        <tr r="B2" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.0525cccb232d485c91876ecb77b7d8b2">
-      <tp t="s">
-        <v>-Calendar</v>
-        <stp/>
-        <stp>-Calendar</stp>
-        <stp>0</stp>
-        <tr r="D4" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.3519a603d24449b7954455d4a9ab6a31">
-      <tp>
-        <v>44178.645821226855</v>
-        <stp/>
-        <stp>Clock</stp>
-        <stp/>
-        <tr r="D9" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.0525cccb232d485c91876ecb77b7d8b2">
-      <tp t="s">
-        <v>DirtyPrice</v>
-        <stp/>
-        <stp>DirtyPrice</stp>
-        <stp>-1893055664</stp>
-        <tr r="D25" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.0525cccb232d485c91876ecb77b7d8b2">
-      <tp t="s">
-        <v>+Tenor</v>
-        <stp/>
-        <stp>+Tenor</stp>
-        <stp>10</stp>
-        <tr r="D10" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.0525cccb232d485c91876ecb77b7d8b2">
-      <tp t="s">
-        <v>Quote</v>
-        <stp/>
-        <stp>Quote</stp>
-        <stp>0</stp>
-        <tr r="D13" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.0525cccb232d485c91876ecb77b7d8b2">
-      <tp t="s">
-        <v>-clock</v>
-        <stp/>
-        <stp>-clock</stp>
-        <stp>-367521373</stp>
-        <tr r="D3" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.3519a603d24449b7954455d4a9ab6a31">
-      <tp>
-        <v>139.26501022498323</v>
-        <stp/>
-        <stp>NPV</stp>
-        <stp/>
-        <tr r="B23" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.0525cccb232d485c91876ecb77b7d8b2">
-      <tp t="s">
-        <v>-PriceDay</v>
-        <stp/>
-        <stp>-PriceDay</stp>
-        <stp>-1100403559</stp>
-        <tr r="D5" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.0525cccb232d485c91876ecb77b7d8b2">
-      <tp t="s">
-        <v>-Schedule</v>
-        <stp/>
-        <stp>-Schedule</stp>
-        <stp>2392593</stp>
-        <tr r="D17" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.3519a603d24449b7954455d4a9ab6a31">
-      <tp>
-        <v>44179</v>
-        <stp/>
-        <stp>-PriceDay</stp>
-        <stp/>
-        <tr r="B5" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.0525cccb232d485c91876ecb77b7d8b2">
-      <tp t="s">
-        <v>Frequency</v>
-        <stp/>
-        <stp>Frequency</stp>
-        <stp>-272257755</stp>
-        <tr r="D12" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.0525cccb232d485c91876ecb77b7d8b2">
-      <tp t="s">
-        <v>-Coupon</v>
-        <stp/>
-        <stp>-Coupon</stp>
-        <stp>561312938</stp>
-        <tr r="D19" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.0525cccb232d485c91876ecb77b7d8b2">
-      <tp t="s">
-        <v>-DayCount</v>
-        <stp/>
-        <stp>-DayCount</stp>
-        <stp>1443484981</stp>
-        <tr r="D6" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.0525cccb232d485c91876ecb77b7d8b2">
-      <tp t="s">
-        <v>NPV</v>
-        <stp/>
-        <stp>NPV</stp>
-        <stp>-1893055664</stp>
-        <tr r="D23" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.0525cccb232d485c91876ecb77b7d8b2">
-      <tp t="s">
-        <v>-Engine</v>
-        <stp/>
-        <stp>-Engine</stp>
-        <stp>2035139617</stp>
-        <tr r="D15" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.0525cccb232d485c91876ecb77b7d8b2">
-      <tp t="s">
-        <v>+Maturity</v>
-        <stp/>
-        <stp>+Maturity</stp>
-        <stp>1718322077</stp>
-        <tr r="D11" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.3519a603d24449b7954455d4a9ab6a31">
-      <tp>
-        <v>177.0109289617487</v>
-        <stp/>
-        <stp>Cash</stp>
-        <stp/>
-        <tr r="B22" s="1"/>
       </tp>
     </main>
   </volType>
@@ -772,7 +772,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -805,7 +805,7 @@
       </c>
       <c r="B2" s="1">
         <f>+_xll._Value(A2)</f>
-        <v>44178</v>
+        <v>44179</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" t="str">
@@ -902,7 +902,7 @@
       </c>
       <c r="D9" s="2">
         <f>+_xll._Clock()</f>
-        <v>44178.645821226855</v>
+        <v>44179.561450185189</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>